<commit_message>
uploading the first data exercise
</commit_message>
<xml_diff>
--- a/Data_Exercises/Data/Variables.xlsx
+++ b/Data_Exercises/Data/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Egyetem\CEU\Fall_Term\Coding_1-Data_Management_and_Analysis_with_R\Coding\Data_Exercises\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7FC181-26F0-48F4-B4EE-C35F14C6C210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21016A6A-E997-4EDB-9752-DC8B0AEDF568}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9FA25332-AFAF-41AE-A449-33D2A4989BF5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Petrol/Diesel/Electric</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Name of the ads</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Age of cars in years</t>
   </si>
 </sst>
 </file>
@@ -496,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED2A785-CA2A-42BF-9FB8-9AD4A4366E6C}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,10 +572,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>21</v>
@@ -577,32 +583,32 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>21</v>
@@ -610,10 +616,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>21</v>
@@ -621,21 +627,21 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>22</v>
@@ -643,10 +649,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>22</v>
@@ -654,23 +660,34 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>